<commit_message>
TODO: Result upload, changelog, feedback
</commit_message>
<xml_diff>
--- a/flaskr/files/Mergebestand.xlsx
+++ b/flaskr/files/Mergebestand.xlsx
@@ -1,92 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timde\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05A4254-C149-482B-B6C7-D335EFB9D989}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{26C45F69-E2FB-4AE2-81D9-646B88E9395D}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12225" windowWidth="24720" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Knummer</t>
-  </si>
-  <si>
-    <t>K23</t>
-  </si>
-  <si>
-    <t>K45</t>
-  </si>
-  <si>
-    <t>K12</t>
-  </si>
-  <si>
-    <t>K56</t>
-  </si>
-  <si>
-    <t>K34</t>
-  </si>
-  <si>
-    <t>Random data</t>
-  </si>
-  <si>
-    <t>Plaats om de data te plaatsen yeet</t>
-  </si>
-  <si>
-    <t>K23 uit Mergebestand yeet1</t>
-  </si>
-  <si>
-    <t>K45 uit Mergebestand neet2</t>
-  </si>
-  <si>
-    <t>K12 uit Mergebestand leet3</t>
-  </si>
-  <si>
-    <t>K56 uit Mergebestand keet4</t>
-  </si>
-  <si>
-    <t>K34 uit Mergebestand heet5</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,24 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -419,76 +351,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E2FB0-2BAB-4CCA-B040-6E491E33C55F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="13.85546875"/>
+    <col customWidth="1" max="2" min="2" width="29.5703125"/>
+    <col customWidth="1" max="3" min="3" width="37.7109375"/>
+    <col customWidth="1" max="4" min="4" width="9.28515625"/>
+    <col customWidth="1" max="5" min="5" width="10.42578125"/>
+    <col customWidth="1" max="6" min="6" width="13.7109375"/>
+    <col customWidth="1" max="8" min="8" width="18.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Knummer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Random data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Random data</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>K23</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>K23 uit Mergebestand yeet1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>K23 uit Mergebestand reet2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>K45</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>K45 uit Mergebestand neet2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>K45 uit Mergebestand qeet4</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>K12</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>K12 uit Mergebestand leet3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>K12 uit Mergebestand oeet1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>K56</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>K56 uit Mergebestand keet4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>K56 uit Mergebestand meet5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>K34</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>K34 uit Mergebestand heet5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>K34 uit Mergebestand weet3</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>